<commit_message>
Added Micro-Mobility Codes to the Cause of Injury List Added Buprenorphine to the Medications List
</commit_message>
<xml_diff>
--- a/DefinedLists/CauseOfInjury/CauseOfInjury.xlsx
+++ b/DefinedLists/CauseOfInjury/CauseOfInjury.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NEMSIS\NEMSIS V3\Suggested Lists_Final for v3.5.0\Most Current Defined Lists on Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\NEMSIS\NEMSIS V3\Defined and Suggested Lists for v3.5.0\Defined and Suggested Lists Most Current\Defined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC1460B7-8DE3-40F0-ABF4-00F38A6B71A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{3A49C271-5FA9-4815-926C-9372EE42022D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recommendation" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="261">
   <si>
     <t/>
   </si>
@@ -787,6 +787,27 @@
   </si>
   <si>
     <t>eInjury.01: Cause of Injury Defined List</t>
+  </si>
+  <si>
+    <t>Electric Bike</t>
+  </si>
+  <si>
+    <t>V29.91</t>
+  </si>
+  <si>
+    <t>Electric (assisted) bicycle rider (driver) (passenger) injured in unspecified traffic accident</t>
+  </si>
+  <si>
+    <t>Electric scooters/boards/skates</t>
+  </si>
+  <si>
+    <t>V00.84</t>
+  </si>
+  <si>
+    <t>Accident with standing micro-mobility pedestrian conveyance</t>
+  </si>
+  <si>
+    <t>Added July 2024</t>
   </si>
 </sst>
 </file>
@@ -921,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1009,6 +1030,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1290,22 +1314,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <pane ySplit="4" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="54.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" customWidth="1"/>
-    <col min="4" max="4" width="94.1796875" customWidth="1"/>
-    <col min="5" max="5" width="55.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="94.140625" customWidth="1"/>
+    <col min="5" max="5" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="33" t="s">
         <v>253</v>
@@ -1313,7 +1338,7 @@
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1321,13 +1346,13 @@
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>242</v>
       </c>
@@ -1344,7 +1369,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>3</v>
       </c>
@@ -1359,7 +1384,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="17" t="s">
         <v>7</v>
@@ -1372,14 +1397,14 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="32"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="19"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>9</v>
       </c>
@@ -1394,7 +1419,7 @@
       </c>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="17" t="s">
         <v>15</v>
@@ -1407,7 +1432,7 @@
       </c>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
       <c r="B10" s="17" t="s">
         <v>12</v>
@@ -1420,14 +1445,14 @@
       </c>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="19"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>17</v>
       </c>
@@ -1442,7 +1467,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
       <c r="B13" s="16" t="s">
         <v>19</v>
@@ -1455,14 +1480,14 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>24</v>
       </c>
@@ -1477,7 +1502,7 @@
       </c>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
       <c r="B16" s="16" t="s">
         <v>32</v>
@@ -1490,7 +1515,7 @@
       </c>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="16" t="s">
         <v>35</v>
@@ -1503,7 +1528,7 @@
       </c>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
       <c r="B18" s="16" t="s">
         <v>29</v>
@@ -1516,14 +1541,14 @@
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="32"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="19"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>37</v>
       </c>
@@ -1538,7 +1563,7 @@
       </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="16" t="s">
         <v>41</v>
@@ -1551,7 +1576,7 @@
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="22" t="s">
         <v>43</v>
@@ -1564,14 +1589,14 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="32"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="19"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>44</v>
       </c>
@@ -1586,7 +1611,7 @@
       </c>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="15" t="s">
         <v>58</v>
@@ -1599,7 +1624,7 @@
       </c>
       <c r="E25" s="10"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="15" t="s">
         <v>93</v>
@@ -1612,7 +1637,7 @@
       </c>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="15" t="s">
         <v>61</v>
@@ -1625,7 +1650,7 @@
       </c>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="B28" s="15" t="s">
         <v>46</v>
@@ -1638,7 +1663,7 @@
       </c>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="15" t="s">
         <v>70</v>
@@ -1651,7 +1676,7 @@
       </c>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="15" t="s">
         <v>73</v>
@@ -1664,7 +1689,7 @@
       </c>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="15" t="s">
         <v>76</v>
@@ -1677,7 +1702,7 @@
       </c>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="15" t="s">
         <v>64</v>
@@ -1690,7 +1715,7 @@
       </c>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="31"/>
       <c r="B33" s="15" t="s">
         <v>49</v>
@@ -1703,7 +1728,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="15" t="s">
         <v>84</v>
@@ -1716,7 +1741,7 @@
       </c>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
       <c r="B35" s="15" t="s">
         <v>81</v>
@@ -1729,7 +1754,7 @@
       </c>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="15" t="s">
         <v>90</v>
@@ -1742,7 +1767,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="15" t="s">
         <v>67</v>
@@ -1755,7 +1780,7 @@
       </c>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
       <c r="B38" s="15" t="s">
         <v>78</v>
@@ -1768,7 +1793,7 @@
       </c>
       <c r="E38" s="10"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="15" t="s">
         <v>87</v>
@@ -1783,7 +1808,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="31"/>
       <c r="B40" s="15" t="s">
         <v>52</v>
@@ -1796,14 +1821,14 @@
       </c>
       <c r="E40" s="10"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
       <c r="D41" s="19"/>
       <c r="E41" s="10"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>95</v>
       </c>
@@ -1820,7 +1845,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="16" t="s">
         <v>119</v>
@@ -1833,7 +1858,7 @@
       </c>
       <c r="E43" s="11"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="16" t="s">
         <v>121</v>
@@ -1846,7 +1871,7 @@
       </c>
       <c r="E44" s="10"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="16" t="s">
         <v>113</v>
@@ -1859,7 +1884,7 @@
       </c>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
       <c r="B46" s="16" t="s">
         <v>116</v>
@@ -1872,7 +1897,7 @@
       </c>
       <c r="E46" s="10"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="16" t="s">
         <v>123</v>
@@ -1885,7 +1910,7 @@
       </c>
       <c r="E47" s="10"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="16" t="s">
         <v>105</v>
@@ -1898,7 +1923,7 @@
       </c>
       <c r="E48" s="10"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="15" t="s">
         <v>99</v>
@@ -1911,7 +1936,7 @@
       </c>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="15" t="s">
         <v>102</v>
@@ -1924,7 +1949,7 @@
       </c>
       <c r="E50" s="10"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="16" t="s">
         <v>110</v>
@@ -1937,7 +1962,7 @@
       </c>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="16" t="s">
         <v>108</v>
@@ -1950,7 +1975,7 @@
       </c>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="15" t="s">
         <v>97</v>
@@ -1963,14 +1988,14 @@
       </c>
       <c r="E53" s="10"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="32"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
       <c r="D54" s="19"/>
       <c r="E54" s="10"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>125</v>
       </c>
@@ -1985,14 +2010,14 @@
       </c>
       <c r="E55" s="10"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="32"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
       <c r="D56" s="19"/>
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>128</v>
       </c>
@@ -2007,7 +2032,7 @@
       </c>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="31"/>
       <c r="B58" s="15" t="s">
         <v>136</v>
@@ -2020,7 +2045,7 @@
       </c>
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="31"/>
       <c r="B59" s="15" t="s">
         <v>139</v>
@@ -2033,7 +2058,7 @@
       </c>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="31"/>
       <c r="B60" s="23" t="s">
         <v>133</v>
@@ -2046,14 +2071,14 @@
       </c>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="32"/>
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
       <c r="D61" s="19"/>
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>243</v>
       </c>
@@ -2068,7 +2093,7 @@
       </c>
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="30"/>
       <c r="B63" s="15" t="s">
         <v>145</v>
@@ -2081,7 +2106,7 @@
       </c>
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="30"/>
       <c r="B64" s="24" t="s">
         <v>142</v>
@@ -2094,7 +2119,7 @@
       </c>
       <c r="E64" s="10"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="30"/>
       <c r="B65" s="15" t="s">
         <v>151</v>
@@ -2107,14 +2132,14 @@
       </c>
       <c r="E65" s="10"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20"/>
       <c r="D66" s="19"/>
       <c r="E66" s="10"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="31" t="s">
         <v>244</v>
       </c>
@@ -2129,7 +2154,7 @@
       </c>
       <c r="E67" s="10"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="31"/>
       <c r="B68" s="15" t="s">
         <v>169</v>
@@ -2142,7 +2167,7 @@
       </c>
       <c r="E68" s="10"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
       <c r="B69" s="15" t="s">
         <v>160</v>
@@ -2155,7 +2180,7 @@
       </c>
       <c r="E69" s="10"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="31"/>
       <c r="B70" s="15" t="s">
         <v>184</v>
@@ -2168,7 +2193,7 @@
       </c>
       <c r="E70" s="10"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
       <c r="B71" s="15" t="s">
         <v>181</v>
@@ -2181,7 +2206,7 @@
       </c>
       <c r="E71" s="10"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="31"/>
       <c r="B72" s="15" t="s">
         <v>178</v>
@@ -2194,7 +2219,7 @@
       </c>
       <c r="E72" s="10"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
       <c r="B73" s="26" t="s">
         <v>189</v>
@@ -2209,7 +2234,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="31"/>
       <c r="B74" s="15" t="s">
         <v>187</v>
@@ -2222,7 +2247,7 @@
       </c>
       <c r="E74" s="10"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="31"/>
       <c r="B75" s="15" t="s">
         <v>166</v>
@@ -2235,7 +2260,7 @@
       </c>
       <c r="E75" s="10"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="31"/>
       <c r="B76" s="15" t="s">
         <v>157</v>
@@ -2248,7 +2273,7 @@
       </c>
       <c r="E76" s="10"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="31"/>
       <c r="B77" s="15" t="s">
         <v>154</v>
@@ -2261,7 +2286,7 @@
       </c>
       <c r="E77" s="10"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="31"/>
       <c r="B78" s="15" t="s">
         <v>163</v>
@@ -2274,7 +2299,7 @@
       </c>
       <c r="E78" s="10"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="31"/>
       <c r="B79" s="15" t="s">
         <v>240</v>
@@ -2289,7 +2314,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="31"/>
       <c r="B80" s="15" t="s">
         <v>175</v>
@@ -2302,14 +2327,14 @@
       </c>
       <c r="E80" s="10"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="32"/>
       <c r="B81" s="20"/>
       <c r="C81" s="20"/>
       <c r="D81" s="19"/>
       <c r="E81" s="10"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="31" t="s">
         <v>35</v>
       </c>
@@ -2324,7 +2349,7 @@
       </c>
       <c r="E82" s="10"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="31"/>
       <c r="B83" s="15" t="s">
         <v>191</v>
@@ -2337,7 +2362,7 @@
       </c>
       <c r="E83" s="10"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="31"/>
       <c r="B84" s="15" t="s">
         <v>195</v>
@@ -2350,7 +2375,7 @@
       </c>
       <c r="E84" s="10"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="31"/>
       <c r="B85" s="16" t="s">
         <v>193</v>
@@ -2363,14 +2388,14 @@
       </c>
       <c r="E85" s="10"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="32"/>
       <c r="B86" s="20"/>
       <c r="C86" s="20"/>
       <c r="D86" s="19"/>
       <c r="E86" s="10"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="31" t="s">
         <v>198</v>
       </c>
@@ -2385,7 +2410,7 @@
       </c>
       <c r="E87" s="10"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="31"/>
       <c r="B88" s="15" t="s">
         <v>203</v>
@@ -2398,165 +2423,195 @@
       </c>
       <c r="E88" s="10"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="32"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="10"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="31" t="s">
+    <row r="89" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="30"/>
+      <c r="B89" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="D89" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="32"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="10"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B91" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="C90" s="15" t="s">
+      <c r="C91" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="D90" s="22" t="s">
+      <c r="D91" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="E90" s="10"/>
-    </row>
-    <row r="91" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="31"/>
-      <c r="B91" s="15" t="s">
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="31"/>
+      <c r="B92" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C92" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="D91" s="15" t="s">
+      <c r="D92" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="E91" s="10"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="32"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="19"/>
       <c r="E92" s="10"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="30" t="s">
+    <row r="93" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="30"/>
+      <c r="B93" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="E93" s="34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="32"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="10"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B95" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="C95" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D93" s="22" t="s">
+      <c r="D95" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="E93" s="10"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="30"/>
-      <c r="B94" s="15" t="s">
+      <c r="E95" s="10"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="30"/>
+      <c r="B96" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C96" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="D94" s="22" t="s">
+      <c r="D96" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="E94" s="10"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="30"/>
-      <c r="B95" s="15" t="s">
+      <c r="E96" s="10"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="30"/>
+      <c r="B97" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C95" s="15" t="s">
+      <c r="C97" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="D95" s="22" t="s">
+      <c r="D97" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E95" s="10"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="32"/>
-      <c r="B96" s="20"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="10"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="31" t="s">
+      <c r="E97" s="10"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="32"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="10"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B99" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C99" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D97" s="23" t="s">
+      <c r="D99" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="E97" s="10"/>
-    </row>
-    <row r="98" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="31"/>
-      <c r="B98" s="15" t="s">
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="31"/>
+      <c r="B100" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C98" s="15" t="s">
+      <c r="C100" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="D98" s="15" t="s">
+      <c r="D100" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="E98" s="10"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="31"/>
-      <c r="B99" s="15" t="s">
+      <c r="E100" s="10"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="31"/>
+      <c r="B101" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C99" s="15" t="s">
+      <c r="C101" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="D99" s="22" t="s">
+      <c r="D101" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="E99" s="10"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="32"/>
-      <c r="B100" s="20"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="19"/>
-      <c r="E100" s="10"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="31" t="s">
+      <c r="E101" s="10"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="32"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="10"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B103" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="C101" s="15" t="s">
+      <c r="C103" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="D101" s="23" t="s">
+      <c r="D103" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="E101" s="10"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="30"/>
-      <c r="B102" s="12"/>
-      <c r="C102" s="12"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="10"/>
+      <c r="E103" s="10"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="30"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="10"/>
     </row>
   </sheetData>
   <sortState ref="B9:D10">

</xml_diff>